<commit_message>
Logik asjustment exchange function
</commit_message>
<xml_diff>
--- a/data/exchangerates.xlsx
+++ b/data/exchangerates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom/Repos/github.com/datachalet/swiss-inflation-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95540C61-2F61-9646-9958-41085BD3E779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F44B6BB-F1D2-EE45-9A1E-0B91046364BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{9AFCE039-1916-2E44-BD6B-2C1DB331A01C}"/>
+    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{9AFCE039-1916-2E44-BD6B-2C1DB331A01C}"/>
   </bookViews>
   <sheets>
     <sheet name="CHF_EUR" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="CHF_XBT" sheetId="3" r:id="rId4"/>
     <sheet name="CHF_XAU" sheetId="4" r:id="rId5"/>
     <sheet name="CHF_GBP" sheetId="5" r:id="rId6"/>
+    <sheet name="CHF_TRY" sheetId="7" r:id="rId7"/>
+    <sheet name="CHF_XAG" sheetId="9" r:id="rId8"/>
+    <sheet name="Quelle" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Year</t>
   </si>
@@ -98,6 +101,27 @@
   </si>
   <si>
     <t>Min CHF/CHF</t>
+  </si>
+  <si>
+    <t>Min CHF/TRY</t>
+  </si>
+  <si>
+    <t>Max CHF/TRY</t>
+  </si>
+  <si>
+    <t>Average CHF/TRY</t>
+  </si>
+  <si>
+    <t>https://fxtop.com/</t>
+  </si>
+  <si>
+    <t>Average CHF/XAG</t>
+  </si>
+  <si>
+    <t>Min CHF/XAG</t>
+  </si>
+  <si>
+    <t>Max CHF/XAG</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC742907-5B53-244D-9261-80905B7A9E19}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="A20:E21"/>
     </sheetView>
   </sheetViews>
@@ -2670,7 +2694,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -3636,7 +3661,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4341,4 +4366,1182 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4351B90D-11FD-2046-A55A-F31C7C4DD210}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B2" s="2">
+        <v>17.372895</v>
+      </c>
+      <c r="C2" s="2">
+        <v>14.351210999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>20.275109</v>
+      </c>
+      <c r="E2" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9.7707739999999994</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7.7546400000000002</v>
+      </c>
+      <c r="D3" s="2">
+        <v>19.257686</v>
+      </c>
+      <c r="E3" s="2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="2">
+        <v>7.5200589999999998</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6.0245800000000003</v>
+      </c>
+      <c r="D4" s="2">
+        <v>9.5009359999999994</v>
+      </c>
+      <c r="E4" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5.7169509999999999</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5.1979709999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6.1583750000000004</v>
+      </c>
+      <c r="E5" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4.953436</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.8239109999999998</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.9369379999999996</v>
+      </c>
+      <c r="E6" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3.704634</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.4622350000000002</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.0193989999999999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3.0677349999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.8600680000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.5110220000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2.8339970000000001</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.2377189999999998</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.1601240000000002</v>
+      </c>
+      <c r="E9" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2.392703</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.2896550000000002</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.6018279999999998</v>
+      </c>
+      <c r="E10" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2.058065</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.87727</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2.4406569999999999</v>
+      </c>
+      <c r="E11" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.9194450000000001</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.822927</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.011409</v>
+      </c>
+      <c r="E12" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.904271</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.595181</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.4145159999999999</v>
+      </c>
+      <c r="E13" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.4483379999999999</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.353556</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.65499</v>
+      </c>
+      <c r="E14" s="2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.4326270000000001</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.348781</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.556071</v>
+      </c>
+      <c r="E15" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.20313</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.036602</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.487406</v>
+      </c>
+      <c r="E16" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.087988</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.0005999999999999</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1.1905619999999999</v>
+      </c>
+      <c r="E17" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.1498870000000001</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.99386399999999997</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1.3640429999999999</v>
+      </c>
+      <c r="E18" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.083194</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.021172</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.1803840000000001</v>
+      </c>
+      <c r="E19" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1.1517120000000001</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.0121089999999999</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.25698</v>
+      </c>
+      <c r="E20" s="2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.1155999999999999</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.975356</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1.2711859999999999</v>
+      </c>
+      <c r="E21" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.98160400000000003</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.76652500000000001</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.1966399999999999</v>
+      </c>
+      <c r="E22" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.73278699999999997</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.40646199999999999</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.017477</v>
+      </c>
+      <c r="E23" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.36908200000000002</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.33840199999999998</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.410024</v>
+      </c>
+      <c r="E24" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>1999</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.30623600000000001</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.270177</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.33973799999999998</v>
+      </c>
+      <c r="E25" s="2">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E5CE84-BBDB-5140-A235-A7914670A13C}">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.5165059999999999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.2805409999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.782659</v>
+      </c>
+      <c r="E2" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.359753</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.188706</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.5517160000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.678193</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.1700950000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2.663049</v>
+      </c>
+      <c r="E4" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.940221</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.6299539999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.1575319999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.0334349999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.8213299999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.2787289999999998</v>
+      </c>
+      <c r="E6" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.858598</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.67286</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.084854</v>
+      </c>
+      <c r="E7" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.8604339999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.549952</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.253768</v>
+      </c>
+      <c r="E8" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2.0668890000000002</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.786659</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.3107790000000001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.7905549999999999</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.587224</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.105785</v>
+      </c>
+      <c r="E10" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.4464440000000001</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.032243</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.8035509999999999</v>
+      </c>
+      <c r="E11" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.0699939999999999</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.93668499999999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.213255</v>
+      </c>
+      <c r="E12" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.0106869999999999</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.72854099999999999</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.242367</v>
+      </c>
+      <c r="E13" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.5178039999999999</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.0425979999999999</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.9367840000000001</v>
+      </c>
+      <c r="E14" s="2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.982656</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.6163609999999999</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2.6434199999999999</v>
+      </c>
+      <c r="E15" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2.0135610000000002</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.4623029999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3.0336850000000002</v>
+      </c>
+      <c r="E16" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.9420120000000001</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.7386680000000001</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2.2188590000000001</v>
+      </c>
+      <c r="E17" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2.1817500000000001</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.7010259999999999</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2.7571720000000002</v>
+      </c>
+      <c r="E18" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3.4419759999999999</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2.641</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4.1690519999999998</v>
+      </c>
+      <c r="E19" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3.7970079999999999</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2.9253119999999999</v>
+      </c>
+      <c r="D20" s="2">
+        <v>4.3662640000000001</v>
+      </c>
+      <c r="E20" s="2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4.7599809999999998</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4.2132750000000003</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5.3156800000000004</v>
+      </c>
+      <c r="E21" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4.366085</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.8918940000000002</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4.89419</v>
+      </c>
+      <c r="E22" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4.2292730000000001</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3.8035770000000002</v>
+      </c>
+      <c r="D23" s="2">
+        <v>4.6480600000000001</v>
+      </c>
+      <c r="E23" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3.724259</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3.4256549999999999</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.148549</v>
+      </c>
+      <c r="E24" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>1999</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3.9808789999999998</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.5828899999999999</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4.6227999999999998</v>
+      </c>
+      <c r="E25" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>1998</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3.9430939999999999</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2.8292519999999999</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.879359</v>
+      </c>
+      <c r="E26" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>1997</v>
+      </c>
+      <c r="B27" s="2">
+        <v>4.4019950000000003</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3.390069</v>
+      </c>
+      <c r="D27" s="2">
+        <v>5.0027020000000002</v>
+      </c>
+      <c r="E27" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>1996</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4.8581640000000004</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4.3933949999999999</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5.2466549999999996</v>
+      </c>
+      <c r="E28" s="2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>1995</v>
+      </c>
+      <c r="B29" s="2">
+        <v>5.078436</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4.3474640000000004</v>
+      </c>
+      <c r="D29" s="2">
+        <v>6.0237249999999998</v>
+      </c>
+      <c r="E29" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>1994</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4.3275810000000003</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3.7619129999999998</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5.1126969999999998</v>
+      </c>
+      <c r="E30" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>1993</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4.9517340000000001</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3.8040039999999999</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5.8594119999999998</v>
+      </c>
+      <c r="E31" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>1992</v>
+      </c>
+      <c r="B32" s="2">
+        <v>5.7274830000000003</v>
+      </c>
+      <c r="C32" s="2">
+        <v>5.093553</v>
+      </c>
+      <c r="D32" s="2">
+        <v>6.7751340000000004</v>
+      </c>
+      <c r="E32" s="2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>1991</v>
+      </c>
+      <c r="B33" s="2">
+        <v>5.3880030000000003</v>
+      </c>
+      <c r="C33" s="2">
+        <v>4.8588040000000001</v>
+      </c>
+      <c r="D33" s="2">
+        <v>6.233816</v>
+      </c>
+      <c r="E33" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>1990</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4.6660769999999996</v>
+      </c>
+      <c r="C34" s="2">
+        <v>4.1036029999999997</v>
+      </c>
+      <c r="D34" s="2">
+        <v>5.1997819999999999</v>
+      </c>
+      <c r="E34" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>1989</v>
+      </c>
+      <c r="B35" s="2">
+        <v>3.4614910000000001</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3.1457269999999999</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3.7895850000000002</v>
+      </c>
+      <c r="E35" s="2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>1988</v>
+      </c>
+      <c r="B36" s="2">
+        <v>3.2646250000000001</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2.960378</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3.7237360000000002</v>
+      </c>
+      <c r="E36" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>1987</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2.9832230000000002</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2.7351549999999998</v>
+      </c>
+      <c r="D37" s="2">
+        <v>3.4687579999999998</v>
+      </c>
+      <c r="E37" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>1986</v>
+      </c>
+      <c r="B38" s="2">
+        <v>3.1820789999999999</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2.7072539999999998</v>
+      </c>
+      <c r="D38" s="2">
+        <v>3.5213960000000002</v>
+      </c>
+      <c r="E38" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>1985</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2.0853429999999999</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1.7304060000000001</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2.44401</v>
+      </c>
+      <c r="E39" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>1984</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1.632369</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1.4735400000000001</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1.812462</v>
+      </c>
+      <c r="E40" s="2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>1983</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1.2957620000000001</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1.2274590000000001</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1.4182729999999999</v>
+      </c>
+      <c r="E41" s="2">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C621BACD-77B1-E540-B524-627EC2B3F514}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>